<commit_message>
fix all but 1 test
</commit_message>
<xml_diff>
--- a/spec/files/0_1_09_no_variables.xlsx
+++ b/spec/files/0_1_09_no_variables.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="12820" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="51200" windowHeight="28260" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outputs!$A$2:$W$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outputs!$A$2:$V$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$W$3</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1699" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1698" uniqueCount="474">
   <si>
     <t>type</t>
   </si>
@@ -4522,9 +4522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B15" sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -5066,56 +5064,53 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB8"/>
+  <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD3"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="61.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="42.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" style="4"/>
-    <col min="10" max="15" width="11.5" style="1"/>
-    <col min="16" max="16" width="46.1640625" style="1" customWidth="1"/>
-    <col min="17" max="19" width="11.5" style="1"/>
-    <col min="20" max="20" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="11.5" style="1"/>
+    <col min="1" max="1" width="45.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="61.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="42.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5" style="4"/>
+    <col min="9" max="14" width="11.5" style="1"/>
+    <col min="15" max="15" width="46.1640625" style="1" customWidth="1"/>
+    <col min="16" max="18" width="11.5" style="1"/>
+    <col min="19" max="19" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="15">
+    <row r="1" spans="1:27" ht="15">
       <c r="A1" s="8" t="s">
         <v>464</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>471</v>
-      </c>
-      <c r="H1" s="8" t="s">
         <v>472</v>
       </c>
+      <c r="H1" s="10"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
@@ -5135,44 +5130,42 @@
       <c r="Y1" s="10"/>
       <c r="Z1" s="10"/>
       <c r="AA1" s="10"/>
-      <c r="AB1" s="10"/>
-    </row>
-    <row r="2" spans="1:28" s="8" customFormat="1" ht="15">
+    </row>
+    <row r="2" spans="1:27" s="8" customFormat="1" ht="15">
       <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
+      <c r="B2" s="10"/>
       <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
+      <c r="D2" s="10" t="s">
+        <v>469</v>
+      </c>
       <c r="E2" s="10" t="s">
-        <v>469</v>
-      </c>
-      <c r="F2" s="10" t="s">
         <v>470</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="10" t="s">
+      <c r="F2" s="15"/>
+      <c r="G2" s="10" t="s">
         <v>473</v>
       </c>
-      <c r="I2" s="9"/>
-    </row>
-    <row r="3" spans="1:28" s="14" customFormat="1" ht="15">
+      <c r="H2" s="9"/>
+    </row>
+    <row r="3" spans="1:27" s="14" customFormat="1" ht="15">
+      <c r="A3" s="10"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="10"/>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
+      <c r="I3" s="16"/>
       <c r="J3" s="16"/>
       <c r="K3" s="16"/>
       <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
+      <c r="M3" s="10"/>
       <c r="N3" s="10"/>
       <c r="O3" s="10"/>
       <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-    </row>
-    <row r="4" spans="1:28" customFormat="1" ht="15">
+    </row>
+    <row r="4" spans="1:27" customFormat="1" ht="15">
       <c r="A4" s="17"/>
       <c r="B4" s="17"/>
       <c r="C4" s="17"/>
@@ -5181,9 +5174,8 @@
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
       <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-    </row>
-    <row r="5" spans="1:28" customFormat="1" ht="15">
+    </row>
+    <row r="5" spans="1:27" customFormat="1" ht="15">
       <c r="A5" s="17"/>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
@@ -5192,12 +5184,11 @@
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
       <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="1"/>
-    </row>
-    <row r="6" spans="1:28" customFormat="1" ht="15">
+      <c r="K5" s="17"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:27" customFormat="1" ht="15">
       <c r="A6" s="17"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
@@ -5206,9 +5197,8 @@
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
       <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-    </row>
-    <row r="7" spans="1:28" customFormat="1" ht="15">
+    </row>
+    <row r="7" spans="1:27" customFormat="1" ht="15">
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
@@ -5217,9 +5207,8 @@
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
       <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-    </row>
-    <row r="8" spans="1:28" customFormat="1" ht="15">
+    </row>
+    <row r="8" spans="1:27" customFormat="1" ht="15">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -5228,7 +5217,6 @@
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
       <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>